<commit_message>
update all QC tests to new format
</commit_message>
<xml_diff>
--- a/documents/test_data/MarineGEO_Seagrass-Macroalgae_Spreadsheet_v0.4.0_test.xlsx
+++ b/documents/test_data/MarineGEO_Seagrass-Macroalgae_Spreadsheet_v0.4.0_test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lonnemanm\Documents\Repositories\data_portal\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlonn\Documents\Repositories\data_portal\documents\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32CF59AE-B8FF-4573-A1A9-75C724DDB692}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2890FCD5-B733-4D39-95ED-D53ECBC8DB28}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="protocol_metadata" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="100">
   <si>
     <t>sheet</t>
   </si>
@@ -398,6 +398,9 @@
   </si>
   <si>
     <t>TEST</t>
+  </si>
+  <si>
+    <t>bonjour</t>
   </si>
 </sst>
 </file>
@@ -1866,7 +1869,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H36" sqref="H36"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1908,8 +1911,8 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="15">
-        <v>43624</v>
+      <c r="A2" s="15" t="s">
+        <v>99</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>98</v>

</xml_diff>